<commit_message>
This project will extract the result form the 3 tested version and make a summary of the result.
Release 1.0
</commit_message>
<xml_diff>
--- a/inputFile/Result.xlsx
+++ b/inputFile/Result.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\z_Sodius\01.AUTOSAR\03.RhpModelisation\Perftesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\JB\git\project.autosar.test.anthi.reg\inputFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D520F-B49A-47ED-85EB-6CC5215C3FDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7CBE1F-8E97-43AE-B2F0-AEEBCCD0C42C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EA1CED3D-D641-4008-A82B-A036D23FFC2F}"/>
   </bookViews>
   <sheets>
-    <sheet name="901" sheetId="1" r:id="rId1"/>
+    <sheet name="05_06_2020" sheetId="3" r:id="rId1"/>
+    <sheet name="04_06_2020" sheetId="1" r:id="rId2"/>
+    <sheet name="01_06_2020" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>migration</t>
   </si>
@@ -56,6 +58,9 @@
   <si>
     <t>Milliseconds</t>
   </si>
+  <si>
+    <t>ECUExtract</t>
+  </si>
 </sst>
 </file>
 
@@ -78,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -247,11 +252,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -268,6 +312,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,25 +628,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26F458F-B6F5-4465-9A21-FEBBCEA57680}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DB9520-5A66-4932-BEB1-8CF3EF3D7ACD}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -619,7 +666,309 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>437073</v>
+      </c>
+      <c r="C3" s="1">
+        <v>458570</v>
+      </c>
+      <c r="D3" s="6">
+        <v>392050</v>
+      </c>
+      <c r="F3" s="5">
+        <f>((D3-C3)*100)/D3</f>
+        <v>-16.967223568422394</v>
+      </c>
+      <c r="G3" s="6">
+        <f>((D3-B3)*100)/D3</f>
+        <v>-11.483994388470858</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>93653</v>
+      </c>
+      <c r="C4" s="1">
+        <v>111864</v>
+      </c>
+      <c r="D4" s="6">
+        <v>111864</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F7" si="0">((D4-C4)*100)/D4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" ref="G4:G7" si="1">((D4-B4)*100)/D4</f>
+        <v>16.279589501537583</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>350328</v>
+      </c>
+      <c r="C5" s="1">
+        <v>240462</v>
+      </c>
+      <c r="D5" s="6">
+        <v>226860</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>-5.9957683152605128</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="1"/>
+        <v>-54.424755355725999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1025</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1025</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1030</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>38053</v>
+      </c>
+      <c r="C7" s="8">
+        <v>137540</v>
+      </c>
+      <c r="D7" s="9">
+        <v>125822</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="0"/>
+        <v>-9.3131566816613951</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="1"/>
+        <v>69.756481378455277</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26F458F-B6F5-4465-9A21-FEBBCEA57680}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>841</v>
+      </c>
+      <c r="C2" s="3">
+        <v>90</v>
+      </c>
+      <c r="D2" s="4">
+        <v>901</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>437073</v>
+      </c>
+      <c r="C3" s="1">
+        <v>458570</v>
+      </c>
+      <c r="D3" s="6">
+        <v>392050</v>
+      </c>
+      <c r="F3" s="5">
+        <f>((D3-C3)*100)/D3</f>
+        <v>-16.967223568422394</v>
+      </c>
+      <c r="G3" s="6">
+        <f>((D3-B3)*100)/D3</f>
+        <v>-11.483994388470858</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>93653</v>
+      </c>
+      <c r="C4" s="1">
+        <v>111864</v>
+      </c>
+      <c r="D4" s="6">
+        <v>111864</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F7" si="0">((D4-C4)*100)/D4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" ref="G4:G7" si="1">((D4-B4)*100)/D4</f>
+        <v>16.279589501537583</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>350328</v>
+      </c>
+      <c r="C5" s="1">
+        <v>240462</v>
+      </c>
+      <c r="D5" s="6">
+        <v>226860</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>-5.9957683152605128</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="1"/>
+        <v>-54.424755355725999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1025</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1025</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1030</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>38053</v>
+      </c>
+      <c r="C7" s="8">
+        <v>137540</v>
+      </c>
+      <c r="D7" s="9">
+        <v>125822</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="0"/>
+        <v>-9.3131566816613951</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="1"/>
+        <v>69.756481378455277</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B87839-DC29-4747-BDC9-C04D5AA03B4A}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>841</v>
+      </c>
+      <c r="C2" s="3">
+        <v>90</v>
+      </c>
+      <c r="D2" s="4">
+        <v>901</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -641,12 +990,12 @@
         <v>-35.432544149397501</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>117126</v>
+        <v>93653</v>
       </c>
       <c r="C4" s="1">
         <v>101146</v>
@@ -655,54 +1004,70 @@
         <v>97356</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" ref="F4:F6" si="0">((D4-C4)*100)/D4</f>
+        <f t="shared" ref="F4:F7" si="0">((D4-C4)*100)/D4</f>
         <v>-3.8929290439212787</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G4:G6" si="1">((D4-B4)*100)/D4</f>
-        <v>-20.306914828053742</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <f t="shared" ref="G4:G7" si="1">((D4-B4)*100)/D4</f>
+        <v>3.8035662927811331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>341867</v>
+        <v>350328</v>
       </c>
       <c r="C5" s="1">
-        <v>242915</v>
+        <v>240462</v>
       </c>
       <c r="D5" s="6">
-        <v>239186</v>
+        <v>226860</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>-1.55903773632236</v>
+        <v>-5.9957683152605128</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" si="1"/>
-        <v>-42.929352052377645</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+        <v>-54.424755355725999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1025</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1025</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1030</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B7" s="8">
         <v>38053</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C7" s="8">
         <v>137540</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D7" s="9">
         <v>125822</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>-9.3131566816613951</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G7" s="9">
         <f t="shared" si="1"/>
         <v>69.756481378455277</v>
       </c>

</xml_diff>